<commit_message>
CHANGED ROW#1 IN THE XLS FILE.
</commit_message>
<xml_diff>
--- a/Mars Share Skill & Manage Listings Test Conditions and Test cases .xlsx
+++ b/Mars Share Skill & Manage Listings Test Conditions and Test cases .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\marsframework-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Marsframework-Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B0FCFC3-6E23-47A3-82F3-DF569F9023DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E205B014-3348-40E6-A4FC-D3862F86B3BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="277">
   <si>
     <t>ID</t>
   </si>
@@ -2236,6 +2236,9 @@
       </rPr>
       <t xml:space="preserve"> Login with Valid Credentials Username:  janakiu3@gmail.com Password:w1nner</t>
     </r>
+  </si>
+  <si>
+    <t>User Should be able to Navigate to the Home pages.</t>
   </si>
 </sst>
 </file>
@@ -7386,12 +7389,72 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="B80:B85"/>
-    <mergeCell ref="A80:A85"/>
-    <mergeCell ref="B87:B93"/>
-    <mergeCell ref="A87:A93"/>
-    <mergeCell ref="A95:A100"/>
-    <mergeCell ref="B95:B100"/>
+    <mergeCell ref="B289:B293"/>
+    <mergeCell ref="A289:A293"/>
+    <mergeCell ref="B283:B287"/>
+    <mergeCell ref="A283:A287"/>
+    <mergeCell ref="B264:B268"/>
+    <mergeCell ref="A264:A268"/>
+    <mergeCell ref="B270:B275"/>
+    <mergeCell ref="A270:A275"/>
+    <mergeCell ref="A277:A281"/>
+    <mergeCell ref="B277:B281"/>
+    <mergeCell ref="A244:A248"/>
+    <mergeCell ref="B244:B248"/>
+    <mergeCell ref="B250:B255"/>
+    <mergeCell ref="A250:A255"/>
+    <mergeCell ref="A257:A262"/>
+    <mergeCell ref="B257:B262"/>
+    <mergeCell ref="B223:B229"/>
+    <mergeCell ref="A223:A229"/>
+    <mergeCell ref="A231:A236"/>
+    <mergeCell ref="B231:B236"/>
+    <mergeCell ref="B238:B242"/>
+    <mergeCell ref="A238:A242"/>
+    <mergeCell ref="B204:B208"/>
+    <mergeCell ref="A204:A208"/>
+    <mergeCell ref="B210:B214"/>
+    <mergeCell ref="A210:A214"/>
+    <mergeCell ref="B216:B221"/>
+    <mergeCell ref="A216:A221"/>
+    <mergeCell ref="A183:A188"/>
+    <mergeCell ref="B183:B188"/>
+    <mergeCell ref="A190:A195"/>
+    <mergeCell ref="B190:B195"/>
+    <mergeCell ref="B197:B202"/>
+    <mergeCell ref="A197:A202"/>
+    <mergeCell ref="B162:B167"/>
+    <mergeCell ref="A162:A167"/>
+    <mergeCell ref="B169:B174"/>
+    <mergeCell ref="A169:A174"/>
+    <mergeCell ref="B176:B181"/>
+    <mergeCell ref="A176:A181"/>
+    <mergeCell ref="B144:B148"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A150:A154"/>
+    <mergeCell ref="B150:B154"/>
+    <mergeCell ref="B156:B160"/>
+    <mergeCell ref="A156:A160"/>
+    <mergeCell ref="B126:B130"/>
+    <mergeCell ref="A126:A130"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="B132:B136"/>
+    <mergeCell ref="A138:A142"/>
+    <mergeCell ref="B138:B142"/>
+    <mergeCell ref="B102:B106"/>
+    <mergeCell ref="A102:A106"/>
+    <mergeCell ref="A120:A124"/>
+    <mergeCell ref="B114:B118"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="B108:B112"/>
+    <mergeCell ref="A108:A112"/>
+    <mergeCell ref="B120:B124"/>
+    <mergeCell ref="B55:B60"/>
+    <mergeCell ref="A55:A60"/>
+    <mergeCell ref="B62:B69"/>
+    <mergeCell ref="A62:A69"/>
+    <mergeCell ref="B71:B78"/>
+    <mergeCell ref="A71:A78"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B7:B12"/>
@@ -7408,72 +7471,12 @@
     <mergeCell ref="A41:A46"/>
     <mergeCell ref="B34:B39"/>
     <mergeCell ref="A34:A39"/>
-    <mergeCell ref="B55:B60"/>
-    <mergeCell ref="A55:A60"/>
-    <mergeCell ref="B62:B69"/>
-    <mergeCell ref="A62:A69"/>
-    <mergeCell ref="B71:B78"/>
-    <mergeCell ref="A71:A78"/>
-    <mergeCell ref="B102:B106"/>
-    <mergeCell ref="A102:A106"/>
-    <mergeCell ref="A120:A124"/>
-    <mergeCell ref="B114:B118"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="B108:B112"/>
-    <mergeCell ref="A108:A112"/>
-    <mergeCell ref="B120:B124"/>
-    <mergeCell ref="B126:B130"/>
-    <mergeCell ref="A126:A130"/>
-    <mergeCell ref="A132:A136"/>
-    <mergeCell ref="B132:B136"/>
-    <mergeCell ref="A138:A142"/>
-    <mergeCell ref="B138:B142"/>
-    <mergeCell ref="B144:B148"/>
-    <mergeCell ref="A144:A148"/>
-    <mergeCell ref="A150:A154"/>
-    <mergeCell ref="B150:B154"/>
-    <mergeCell ref="B156:B160"/>
-    <mergeCell ref="A156:A160"/>
-    <mergeCell ref="B162:B167"/>
-    <mergeCell ref="A162:A167"/>
-    <mergeCell ref="B169:B174"/>
-    <mergeCell ref="A169:A174"/>
-    <mergeCell ref="B176:B181"/>
-    <mergeCell ref="A176:A181"/>
-    <mergeCell ref="A183:A188"/>
-    <mergeCell ref="B183:B188"/>
-    <mergeCell ref="A190:A195"/>
-    <mergeCell ref="B190:B195"/>
-    <mergeCell ref="B197:B202"/>
-    <mergeCell ref="A197:A202"/>
-    <mergeCell ref="B204:B208"/>
-    <mergeCell ref="A204:A208"/>
-    <mergeCell ref="B210:B214"/>
-    <mergeCell ref="A210:A214"/>
-    <mergeCell ref="B216:B221"/>
-    <mergeCell ref="A216:A221"/>
-    <mergeCell ref="B223:B229"/>
-    <mergeCell ref="A223:A229"/>
-    <mergeCell ref="A231:A236"/>
-    <mergeCell ref="B231:B236"/>
-    <mergeCell ref="B238:B242"/>
-    <mergeCell ref="A238:A242"/>
-    <mergeCell ref="A244:A248"/>
-    <mergeCell ref="B244:B248"/>
-    <mergeCell ref="B250:B255"/>
-    <mergeCell ref="A250:A255"/>
-    <mergeCell ref="A257:A262"/>
-    <mergeCell ref="B257:B262"/>
-    <mergeCell ref="B289:B293"/>
-    <mergeCell ref="A289:A293"/>
-    <mergeCell ref="B283:B287"/>
-    <mergeCell ref="A283:A287"/>
-    <mergeCell ref="B264:B268"/>
-    <mergeCell ref="A264:A268"/>
-    <mergeCell ref="B270:B275"/>
-    <mergeCell ref="A270:A275"/>
-    <mergeCell ref="A277:A281"/>
-    <mergeCell ref="B277:B281"/>
+    <mergeCell ref="B80:B85"/>
+    <mergeCell ref="A80:A85"/>
+    <mergeCell ref="B87:B93"/>
+    <mergeCell ref="A87:A93"/>
+    <mergeCell ref="A95:A100"/>
+    <mergeCell ref="B95:B100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -24134,7 +24137,7 @@
   <dimension ref="A1:H475"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24186,7 +24189,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>96</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -25948,6 +25951,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="A20:A25"/>
     <mergeCell ref="A53:A59"/>
     <mergeCell ref="A61:A67"/>
     <mergeCell ref="A27:A31"/>
@@ -25960,12 +25969,6 @@
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B46:B51"/>
     <mergeCell ref="A46:A51"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="A20:A25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>